<commit_message>
updating the mapping table
</commit_message>
<xml_diff>
--- a/PRIAM Metamodel/Mapping Article-PRIAM.xlsx
+++ b/PRIAM Metamodel/Mapping Article-PRIAM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selena\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\doctorat\Travail personnel\2023\SoSyM revue\Complementary files\PRIAM Metamodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA9A1C8-FD8E-4879-8691-D0D6C68584C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7687B83D-4855-4CE6-8495-FDAD3445FA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{095F3C4A-825F-46E1-BE34-2B4EC481721F}"/>
   </bookViews>
@@ -145,10 +145,6 @@
     <t>In implementation, these elements allow the system to ensure compliance with GDPR principles, supporting transparency, enabling data modification to maintain accuracy, enforcing purpose limitation, and ensuring proper retention and protection of data.</t>
   </si>
   <si>
-    <t>PRIAM  cannot judge whether data collection is excessive or objectively 
-justified in a given context.</t>
-  </si>
-  <si>
     <r>
       <t>Article 6</t>
     </r>
@@ -170,9 +166,6 @@
   </si>
   <si>
     <t>Thanks to this legal basis, the system can manage the rights of both application owner and data subjects regarding the execution of each processing, ensuring compliance with GDPR obligations.</t>
-  </si>
-  <si>
-    <t>PRIAM cannot verify whether that legal basis is valid</t>
   </si>
   <si>
     <r>
@@ -297,10 +290,6 @@
     <t>PRIAM enforces structural consistency by ensuring that rights requests (DataRequest) can only be created for personal data that is linked to a data subject,</t>
   </si>
   <si>
-    <t>PRIAM cannot determine whether a controller is legally exempt from identifying a
- data subject under Article 11, nor can it assess whether additional identification efforts would be reasonable or proportionate; this requires legal and contextual human judgment.</t>
-  </si>
-  <si>
     <t>III</t>
   </si>
   <si>
@@ -518,10 +507,6 @@
     <t>A data subject can submit a portability request via DataRequest, and PRIAM can generate a structured, machine-readable export of the relevant Data and Processing, and record the transfer event.</t>
   </si>
   <si>
-    <t>Direct transmission to another system or handling portability exceptions
- (public-interest processing, third-party rights) requires external tools and human oversight.</t>
-  </si>
-  <si>
     <r>
       <t>Article 21</t>
     </r>
@@ -546,10 +531,6 @@
     <t>Allows registering and tracking objection requests, prevente further execution of the targeted processing, and retains the history of requests (audit case).</t>
   </si>
   <si>
-    <t>Determining whether compelling legitimate grounds override the objection
- or applying exemptions for research/statistics requires legal evaluation and human decision-making.</t>
-  </si>
-  <si>
     <r>
       <t>Article 22</t>
     </r>
@@ -596,10 +577,6 @@
 They can submit a review or objection request via ProcessingRequest, and PRIAM can record it, indicating that human intervention or contestation is required.</t>
   </si>
   <si>
-    <t>PRIAM cannot autonomously assess the legal or significant effects of automated
- decisions, enforce exceptions</t>
-  </si>
-  <si>
     <r>
       <t>Article 23</t>
     </r>
@@ -644,10 +621,6 @@
   </si>
   <si>
     <t xml:space="preserve">PRIAM partially enforces structural accountability through built-in validators (e.g., preventing incomplete processing records) and generates compliance artefacts automatically (records of processing). </t>
-  </si>
-  <si>
-    <t>Evaluating whether measures are actually sufficient or appropriate under
- GDPR requires human assessment.</t>
   </si>
   <si>
     <r>
@@ -701,31 +674,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">PRIAM cannot model or verify the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>legal allocation of obligations</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> between
- joint controllers (e.g. who must inform data subjects, who handles which rights), nor assess whether their arrangement complies with Article 26; this requires human/legal judgment.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Article 27</t>
     </r>
     <r>
@@ -812,9 +760,6 @@
     <t>PRIAM can describe all elements required for records of processing activities by structuring Processing, Purpose, Data, DataSubjectCategory, SecondaryActor, transfers, and measures within the model.</t>
   </si>
   <si>
-    <t>Génération automatique de PRIAM à partir d'information que gère le métamodèle</t>
-  </si>
-  <si>
     <r>
       <t>Article 31</t>
     </r>
@@ -833,10 +778,6 @@
   </si>
   <si>
     <t>PRIAM  describe the supervisory authority as a secondary actor and relate it to processings and breaches.</t>
-  </si>
-  <si>
-    <t>Effective cooperation with the authority involves physical or organizational 
-actions outside of PRIAM.</t>
   </si>
   <si>
     <r>
@@ -927,10 +868,6 @@
     <t>PRIAM describe a DPIA using the DPIA class linked to relevant Processings, showing which personal data, purposes, and measures are involved</t>
   </si>
   <si>
-    <t xml:space="preserve"> An expert evaluation is needed (to judge the adequacy of the risk assessment, 
-evaluate mitigation effectiveness,...).</t>
-  </si>
-  <si>
     <r>
       <t>Article 36</t>
     </r>
@@ -949,9 +886,6 @@
   </si>
   <si>
     <t>PRIAM documents the information necessary for a consultation with the supervisory authority (processing, purposes, DPO, ...) and DPIA is also available.</t>
-  </si>
-  <si>
-    <t>La vérification automatique que la consultation a eu lieu reste hors de portée ; l’action réelle dépend de procédures externes.</t>
   </si>
   <si>
     <t>Article 37 – Designation of the data protection officer (DPO)</t>
@@ -1030,10 +964,6 @@
     <t>PRIAM provides descriptive support only: codes of conduct and certifications can be documented and linked to processings and actors via the Document package</t>
   </si>
   <si>
-    <t>PRIAM can only document references to codes of conduct and certifications, 
-while human intervention is required to assess their legal validity, approval status, scope, and effective application.</t>
-  </si>
-  <si>
     <r>
       <t>Article 41</t>
     </r>
@@ -1109,10 +1039,6 @@
   </si>
   <si>
     <t>PRIAM enforces that any transfer is explicitly recorded and associated with a recipient and data, preventing undocumented transfers in the system.</t>
-  </si>
-  <si>
-    <t>Human intervention is required to determine the legality, proportionality, and
- applicability of transfer mechanisms under GDPR.</t>
   </si>
   <si>
     <r>
@@ -1257,6 +1183,50 @@
   <si>
     <t>Restrictions for processing 
 criminal conviction data</t>
+  </si>
+  <si>
+    <t>Evaluating whether measures are actually sufficient or appropriate under GDPR requires human assessment.</t>
+  </si>
+  <si>
+    <t>PRIAM cannot autonomously assess the legal or significant effects of automated decisions, enforce exceptions</t>
+  </si>
+  <si>
+    <t>Determining whether compelling legitimate grounds override the objection or applying exemptions for research/statistics requires legal evaluation and human decision-making.</t>
+  </si>
+  <si>
+    <t>Effective cooperation with the authority involves physical or organizational  actions outside of PRIAM.</t>
+  </si>
+  <si>
+    <t>Human intervention is required to determine the legality, proportionality, and applicability of transfer mechanisms under GDPR.</t>
+  </si>
+  <si>
+    <t>PRIAM can only document references to codes of conduct and certifications, while human intervention is required to assess their legal validity, approval status, scope, and effective application.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An expert evaluation is needed (to judge the adequacy of the risk assessment, evaluate mitigation effectiveness,...).</t>
+  </si>
+  <si>
+    <t>PRIAM cannot model or verify the legal allocation of obligations between
+ joint controllers (e.g. who must inform data subjects, who handles which rights), nor assess whether their arrangement complies with Article 26; this requires human/legal judgment.</t>
+  </si>
+  <si>
+    <t>PRIAM  cannot judge whether data collection is excessive or objectively justified in a given context.</t>
+  </si>
+  <si>
+    <t>PRIAM cannot determine whether a controller is legally exempt from identifying a data subject under Article 11, nor can it assess whether additional identification efforts would be reasonable or proportionate; this requires legal and contextual human judgment.</t>
+  </si>
+  <si>
+    <t>PRIAM automatically generates the record of processings from information managed by the metamodel</t>
+  </si>
+  <si>
+    <t>PRIAM cannot verify whether that legal basis is valid. 
+Humain intervention is required.</t>
+  </si>
+  <si>
+    <t>Direct transmission to another system or handling portability exceptions (public-interest processing, third-party rights) requires human oversight.</t>
+  </si>
+  <si>
+    <t>Automatic verification that the consultation took place remains out of reach. This requires human intervention.</t>
   </si>
 </sst>
 </file>
@@ -1505,6 +1475,63 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1514,67 +1541,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1899,7 +1869,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F5"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1933,7 +1903,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1942,50 +1912,50 @@
       <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="29"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2001,755 +1971,757 @@
         <v>20</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="C11" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="2" t="s">
+      <c r="D12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="F12" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="D13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="E13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="2" t="s">
+      <c r="E14" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="2" t="s">
+      <c r="E15" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="2" t="s">
+      <c r="E16" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="F16" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="7" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="D17" s="7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="2" t="s">
+      <c r="E17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="30"/>
-    </row>
-    <row r="18" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="2" t="s">
+      <c r="E18" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="F18" s="25"/>
+    </row>
+    <row r="19" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="31"/>
-    </row>
-    <row r="19" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="2" t="s">
+      <c r="E19" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="F19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="7" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="B20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="2" t="s">
+      <c r="E20" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
+      <c r="B21" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="2" t="s">
+      <c r="E21" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="F21" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
+      <c r="B22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="E22" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="2" t="s">
+      <c r="F22" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F23" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+      <c r="B24" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="2" t="s">
+      <c r="C24" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D24" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>99</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
+      <c r="B26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="D26" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="E26" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="7" t="s">
+    </row>
+    <row r="27" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
+      <c r="B27" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="2" t="s">
+      <c r="D27" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="E27" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="F27" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
+      <c r="B28" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="D28" s="7" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7" t="s">
-        <v>134</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+      <c r="A34" s="13"/>
+      <c r="B34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="13"/>
+      <c r="B35" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" s="27"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
+      <c r="B36" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A34" s="17"/>
-      <c r="B34" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="17"/>
-      <c r="B35" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-    </row>
-    <row r="36" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="17"/>
-      <c r="B36" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="13"/>
+      <c r="B37" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="13"/>
+      <c r="B38" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="13"/>
+      <c r="B39" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="28"/>
+    </row>
+    <row r="40" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+      <c r="A40" s="13"/>
+      <c r="B40" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="17"/>
-      <c r="B37" s="2" t="s">
+      <c r="C40" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D40" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="17"/>
-      <c r="B38" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="17"/>
-      <c r="B39" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="16"/>
-    </row>
-    <row r="40" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A40" s="17"/>
-      <c r="B40" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="13"/>
+      <c r="B41" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" s="23"/>
+      <c r="F41" s="28" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="13"/>
+      <c r="B42" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" s="30"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="13"/>
+    </row>
+    <row r="43" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="13"/>
+      <c r="B43" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" s="30"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="13"/>
+    </row>
+    <row r="44" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="13"/>
+      <c r="B44" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" s="31"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="13"/>
+    </row>
+    <row r="45" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="17"/>
-      <c r="B41" s="2" t="s">
+      <c r="D45" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="E45" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="F45" s="28" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="13"/>
+      <c r="B46" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="F41" s="16" t="s">
+      <c r="C46" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
-      <c r="B42" s="2" t="s">
+      <c r="D46" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="E46" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="17"/>
-    </row>
-    <row r="43" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="17"/>
-      <c r="B43" s="2" t="s">
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="13"/>
+      <c r="B47" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="17"/>
-    </row>
-    <row r="44" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="17"/>
-      <c r="B44" s="2" t="s">
+      <c r="D47" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="E47" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="17"/>
-    </row>
-    <row r="45" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="17" t="s">
+      <c r="F47" s="13"/>
+    </row>
+    <row r="48" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="13"/>
+      <c r="B48" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C48" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="D48" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="E48" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="F48" s="13"/>
+    </row>
+    <row r="49" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+      <c r="A49" s="13"/>
+      <c r="B49" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="C49" s="6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="17"/>
-      <c r="B46" s="2" t="s">
+      <c r="D49" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="E49" s="7"/>
+      <c r="F49" s="13"/>
+    </row>
+    <row r="50" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+      <c r="A50" s="13"/>
+      <c r="B50" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="C50" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="D50" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="F46" s="17"/>
-    </row>
-    <row r="47" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="17"/>
-      <c r="B47" s="2" t="s">
+      <c r="E50" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+      <c r="A51" s="13"/>
+      <c r="B51" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="C51" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="F47" s="17"/>
-    </row>
-    <row r="48" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
-      <c r="B48" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F48" s="17"/>
-    </row>
-    <row r="49" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A49" s="17"/>
-      <c r="B49" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="E49" s="7"/>
-      <c r="F49" s="17"/>
-    </row>
-    <row r="50" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A50" s="17"/>
-      <c r="B50" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="F50" s="17"/>
-    </row>
-    <row r="51" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A51" s="17"/>
-      <c r="B51" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>201</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
-      <c r="F51" s="17"/>
+      <c r="F51" s="13"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
+      <c r="A52" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="18"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
+      <c r="A53" s="10"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A45:A51"/>
+    <mergeCell ref="F45:F51"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="B52:C53"/>
     <mergeCell ref="D52:F53"/>
@@ -2766,8 +2738,6 @@
     <mergeCell ref="D41:D44"/>
     <mergeCell ref="E41:E44"/>
     <mergeCell ref="F41:F44"/>
-    <mergeCell ref="A45:A51"/>
-    <mergeCell ref="F45:F51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>